<commit_message>
Edited mutation table to remove "uncommon" mutation rows, following discussion with Markus.
</commit_message>
<xml_diff>
--- a/COLORECTAL_MUTATION_TABLE.xlsx
+++ b/COLORECTAL_MUTATION_TABLE.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="178">
   <si>
     <t>BRAF</t>
   </si>
@@ -536,25 +536,13 @@
     <t>VEP Consequence types are SO terms described at http://www.ensembl.org/info/genome/variation/predicted_data.html#consequences</t>
   </si>
   <si>
-    <t>transcript_ablation, splice_acceptor_variant, splice_donor_variant, stop_gained, frameshift_variant, stop_lost, start_lost, inframe_insertion, inframe_deletion, missense_variant</t>
-  </si>
-  <si>
     <t>Flag</t>
   </si>
   <si>
-    <t>BRAF_UNCOMMON</t>
-  </si>
-  <si>
     <t>BRAF_COMMON</t>
   </si>
   <si>
-    <t>KRAS_UNCOMMOON</t>
-  </si>
-  <si>
     <t>KRAS_COMMON</t>
-  </si>
-  <si>
-    <t>NRAS_UNCOMMON</t>
   </si>
   <si>
     <t>NRAS_COMMON</t>
@@ -655,8 +643,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="169">
+  <cellStyleXfs count="179">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -863,7 +861,7 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="169">
+  <cellStyles count="179">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -948,6 +946,11 @@
     <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1032,6 +1035,11 @@
     <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1365,7 +1373,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1385,7 +1393,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>3</v>
@@ -1394,15 +1402,15 @@
         <v>4</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="2" t="s">
-        <v>171</v>
+        <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -1413,111 +1421,63 @@
       <c r="D2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="10"/>
+      <c r="E2" s="10" t="s">
+        <v>176</v>
+      </c>
       <c r="F2" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="I2"/>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="I2"/>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" s="2" t="s">
+      <c r="I3"/>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>180</v>
-      </c>
-      <c r="F3" s="2" t="s">
+      <c r="B4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="I3"/>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="11"/>
-      <c r="F4" s="3" t="s">
-        <v>175</v>
-      </c>
       <c r="I4"/>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>176</v>
-      </c>
       <c r="I5"/>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="4" t="s">
-        <v>171</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="12"/>
-      <c r="F6" s="4" t="s">
-        <v>177</v>
-      </c>
       <c r="I6"/>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>178</v>
-      </c>
       <c r="I7"/>
     </row>
     <row r="8" spans="1:9">

</xml_diff>

<commit_message>
Mutation table doesn't require colour in formatting.
</commit_message>
<xml_diff>
--- a/COLORECTAL_MUTATION_TABLE.xlsx
+++ b/COLORECTAL_MUTATION_TABLE.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Alascca table of mutation class" sheetId="1" r:id="rId1"/>
+    <sheet name="MutationTable" sheetId="1" r:id="rId1"/>
     <sheet name="Version notes" sheetId="2" r:id="rId2"/>
     <sheet name="consequence_types" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -608,30 +608,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -824,12 +806,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -841,15 +820,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1373,7 +1343,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1381,11 +1351,11 @@
     <col min="1" max="1" width="21.6640625" customWidth="1"/>
     <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="21" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23" style="13" customWidth="1"/>
+    <col min="5" max="5" width="23" style="7" customWidth="1"/>
     <col min="6" max="6" width="18.5" customWidth="1"/>
     <col min="7" max="7" width="20.83203125" customWidth="1"/>
     <col min="8" max="8" width="88.5" customWidth="1"/>
-    <col min="9" max="9" width="99" style="7" customWidth="1"/>
+    <col min="9" max="9" width="99" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1">
@@ -1401,7 +1371,7 @@
       <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="6" t="s">
         <v>175</v>
       </c>
       <c r="F1" s="1" t="s">
@@ -1409,64 +1379,64 @@
       </c>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="2" t="s">
+      <c r="A2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" t="s">
         <v>176</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" t="s">
         <v>172</v>
       </c>
       <c r="I2"/>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="3" t="s">
+      <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" t="s">
         <v>26</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" t="s">
         <v>173</v>
       </c>
       <c r="I3"/>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" s="4" t="s">
+      <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E4" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" t="s">
         <v>174</v>
       </c>
       <c r="I4"/>
@@ -1481,7 +1451,7 @@
       <c r="I7"/>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="7"/>
+      <c r="A8" s="4"/>
       <c r="E8"/>
       <c r="I8"/>
     </row>
@@ -1514,222 +1484,222 @@
       <c r="I15"/>
     </row>
     <row r="16" spans="1:9">
-      <c r="A16" s="6"/>
+      <c r="A16" s="3"/>
       <c r="E16"/>
       <c r="I16"/>
     </row>
     <row r="17" spans="1:9">
-      <c r="A17" s="6"/>
+      <c r="A17" s="3"/>
       <c r="E17"/>
       <c r="I17"/>
     </row>
     <row r="18" spans="1:9">
-      <c r="A18" s="6"/>
+      <c r="A18" s="3"/>
       <c r="E18"/>
       <c r="I18"/>
     </row>
     <row r="19" spans="1:9">
-      <c r="A19" s="6"/>
+      <c r="A19" s="3"/>
       <c r="E19"/>
       <c r="I19"/>
     </row>
     <row r="20" spans="1:9">
-      <c r="A20" s="7"/>
+      <c r="A20" s="4"/>
       <c r="E20"/>
       <c r="I20"/>
     </row>
     <row r="21" spans="1:9">
-      <c r="A21" s="14"/>
+      <c r="A21" s="8"/>
       <c r="E21"/>
       <c r="I21"/>
     </row>
     <row r="22" spans="1:9">
-      <c r="A22" s="14"/>
+      <c r="A22" s="8"/>
       <c r="E22"/>
       <c r="I22"/>
     </row>
     <row r="23" spans="1:9">
-      <c r="A23" s="7"/>
+      <c r="A23" s="4"/>
       <c r="E23"/>
       <c r="I23"/>
     </row>
     <row r="24" spans="1:9">
-      <c r="A24" s="7"/>
+      <c r="A24" s="4"/>
       <c r="E24"/>
       <c r="I24"/>
     </row>
     <row r="25" spans="1:9">
-      <c r="A25" s="7"/>
+      <c r="A25" s="4"/>
       <c r="E25"/>
       <c r="I25"/>
     </row>
     <row r="26" spans="1:9">
-      <c r="A26" s="7"/>
+      <c r="A26" s="4"/>
       <c r="E26"/>
       <c r="I26"/>
     </row>
     <row r="27" spans="1:9">
-      <c r="A27" s="5"/>
+      <c r="A27" s="2"/>
       <c r="E27"/>
       <c r="I27"/>
     </row>
     <row r="28" spans="1:9">
-      <c r="A28" s="7"/>
+      <c r="A28" s="4"/>
       <c r="E28"/>
       <c r="I28"/>
     </row>
     <row r="49" spans="1:1">
-      <c r="A49" s="8"/>
+      <c r="A49" s="5"/>
     </row>
     <row r="50" spans="1:1">
-      <c r="A50" s="8"/>
+      <c r="A50" s="5"/>
     </row>
     <row r="51" spans="1:1">
-      <c r="A51" s="8"/>
+      <c r="A51" s="5"/>
     </row>
     <row r="52" spans="1:1">
-      <c r="A52" s="8"/>
+      <c r="A52" s="5"/>
     </row>
     <row r="53" spans="1:1">
-      <c r="A53" s="8"/>
+      <c r="A53" s="5"/>
     </row>
     <row r="54" spans="1:1">
-      <c r="A54" s="8"/>
+      <c r="A54" s="5"/>
     </row>
     <row r="55" spans="1:1">
-      <c r="A55" s="8"/>
+      <c r="A55" s="5"/>
     </row>
     <row r="56" spans="1:1">
-      <c r="A56" s="8"/>
+      <c r="A56" s="5"/>
     </row>
     <row r="57" spans="1:1">
-      <c r="A57" s="8"/>
+      <c r="A57" s="5"/>
     </row>
     <row r="58" spans="1:1">
-      <c r="A58" s="8"/>
+      <c r="A58" s="5"/>
     </row>
     <row r="59" spans="1:1">
-      <c r="A59" s="8"/>
+      <c r="A59" s="5"/>
     </row>
     <row r="60" spans="1:1">
-      <c r="A60" s="8"/>
+      <c r="A60" s="5"/>
     </row>
     <row r="61" spans="1:1">
-      <c r="A61" s="8"/>
+      <c r="A61" s="5"/>
     </row>
     <row r="62" spans="1:1">
-      <c r="A62" s="8"/>
+      <c r="A62" s="5"/>
     </row>
     <row r="63" spans="1:1">
-      <c r="A63" s="8"/>
+      <c r="A63" s="5"/>
     </row>
     <row r="64" spans="1:1">
-      <c r="A64" s="8"/>
+      <c r="A64" s="5"/>
     </row>
     <row r="65" spans="1:1">
-      <c r="A65" s="8"/>
+      <c r="A65" s="5"/>
     </row>
     <row r="66" spans="1:1">
-      <c r="A66" s="8"/>
+      <c r="A66" s="5"/>
     </row>
     <row r="67" spans="1:1">
-      <c r="A67" s="8"/>
+      <c r="A67" s="5"/>
     </row>
     <row r="68" spans="1:1">
-      <c r="A68" s="8"/>
+      <c r="A68" s="5"/>
     </row>
     <row r="69" spans="1:1">
-      <c r="A69" s="8"/>
+      <c r="A69" s="5"/>
     </row>
     <row r="70" spans="1:1">
-      <c r="A70" s="8"/>
+      <c r="A70" s="5"/>
     </row>
     <row r="71" spans="1:1">
-      <c r="A71" s="8"/>
+      <c r="A71" s="5"/>
     </row>
     <row r="72" spans="1:1">
-      <c r="A72" s="8"/>
+      <c r="A72" s="5"/>
     </row>
     <row r="73" spans="1:1">
-      <c r="A73" s="8"/>
+      <c r="A73" s="5"/>
     </row>
     <row r="74" spans="1:1">
-      <c r="A74" s="8"/>
+      <c r="A74" s="5"/>
     </row>
     <row r="75" spans="1:1">
-      <c r="A75" s="8"/>
+      <c r="A75" s="5"/>
     </row>
     <row r="76" spans="1:1">
-      <c r="A76" s="8"/>
+      <c r="A76" s="5"/>
     </row>
     <row r="77" spans="1:1">
-      <c r="A77" s="8"/>
+      <c r="A77" s="5"/>
     </row>
     <row r="78" spans="1:1">
-      <c r="A78" s="8"/>
+      <c r="A78" s="5"/>
     </row>
     <row r="79" spans="1:1">
-      <c r="A79" s="8"/>
+      <c r="A79" s="5"/>
     </row>
     <row r="80" spans="1:1">
-      <c r="A80" s="8"/>
+      <c r="A80" s="5"/>
     </row>
     <row r="81" spans="1:1">
-      <c r="A81" s="8"/>
+      <c r="A81" s="5"/>
     </row>
     <row r="82" spans="1:1">
-      <c r="A82" s="8"/>
+      <c r="A82" s="5"/>
     </row>
     <row r="83" spans="1:1">
-      <c r="A83" s="8"/>
+      <c r="A83" s="5"/>
     </row>
     <row r="84" spans="1:1">
-      <c r="A84" s="8"/>
+      <c r="A84" s="5"/>
     </row>
     <row r="85" spans="1:1">
-      <c r="A85" s="8"/>
+      <c r="A85" s="5"/>
     </row>
     <row r="86" spans="1:1">
-      <c r="A86" s="8"/>
+      <c r="A86" s="5"/>
     </row>
     <row r="87" spans="1:1">
-      <c r="A87" s="8"/>
+      <c r="A87" s="5"/>
     </row>
     <row r="88" spans="1:1">
-      <c r="A88" s="8"/>
+      <c r="A88" s="5"/>
     </row>
     <row r="89" spans="1:1">
-      <c r="A89" s="8"/>
+      <c r="A89" s="5"/>
     </row>
     <row r="90" spans="1:1">
-      <c r="A90" s="8"/>
+      <c r="A90" s="5"/>
     </row>
     <row r="91" spans="1:1">
-      <c r="A91" s="8"/>
+      <c r="A91" s="5"/>
     </row>
     <row r="92" spans="1:1">
-      <c r="A92" s="8"/>
+      <c r="A92" s="5"/>
     </row>
     <row r="93" spans="1:1">
-      <c r="A93" s="8"/>
+      <c r="A93" s="5"/>
     </row>
     <row r="94" spans="1:1">
-      <c r="A94" s="8"/>
+      <c r="A94" s="5"/>
     </row>
     <row r="95" spans="1:1">
-      <c r="A95" s="8"/>
+      <c r="A95" s="5"/>
     </row>
     <row r="96" spans="1:1">
-      <c r="A96" s="8"/>
+      <c r="A96" s="5"/>
     </row>
     <row r="97" spans="1:1">
-      <c r="A97" s="8"/>
+      <c r="A97" s="5"/>
     </row>
     <row r="98" spans="1:1">
-      <c r="A98" s="8"/>
+      <c r="A98" s="5"/>
     </row>
     <row r="99" spans="1:1">
-      <c r="A99" s="8"/>
+      <c r="A99" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1780,7 +1750,7 @@
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="10" t="s">
         <v>94</v>
       </c>
       <c r="B4" t="s">
@@ -2038,8 +2008,8 @@
       <c r="F13" t="s">
         <v>41</v>
       </c>
-      <c r="T13" s="15"/>
-      <c r="Z13" s="15"/>
+      <c r="T13" s="9"/>
+      <c r="Z13" s="9"/>
     </row>
     <row r="14" spans="1:26">
       <c r="B14" t="s">

</xml_diff>

<commit_message>
Writing tests for selected classes/methods of reports.py, and debugging.
</commit_message>
<xml_diff>
--- a/COLORECTAL_MUTATION_TABLE.xlsx
+++ b/COLORECTAL_MUTATION_TABLE.xlsx
@@ -551,10 +551,10 @@
     <t>Amino_acid_changes</t>
   </si>
   <si>
-    <t>V600E</t>
-  </si>
-  <si>
     <t>Symbol</t>
+  </si>
+  <si>
+    <t>Val600Glu</t>
   </si>
 </sst>
 </file>
@@ -625,8 +625,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="179">
+  <cellStyleXfs count="199">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -831,7 +851,7 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="179">
+  <cellStyles count="199">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -921,6 +941,16 @@
     <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="194" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="196" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="198" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1010,6 +1040,16 @@
     <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="187" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="189" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="191" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="193" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="195" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="197" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1343,7 +1383,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1363,7 +1403,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>3</v>
@@ -1392,7 +1432,7 @@
         <v>2</v>
       </c>
       <c r="E2" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="F2" t="s">
         <v>172</v>

</xml_diff>